<commit_message>
nmv 01 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.3 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56123A54-5F79-4AB2-B2BC-92F7232E7C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83068E72-3FF5-4463-B287-ED4C2F7B7B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3753,9 +3753,6 @@
     <t>sAqddhyeti# sAqddhyA</t>
   </si>
   <si>
-    <t>aqddhvaqryU iti# addhvaqryU</t>
-  </si>
-  <si>
     <t>tveti# tvA</t>
   </si>
   <si>
@@ -4636,6 +4633,9 @@
   </si>
   <si>
     <t>r.  to  add</t>
+  </si>
+  <si>
+    <t>aqddhvaqryU itya#ddhvaqryU</t>
   </si>
 </sst>
 </file>
@@ -4870,7 +4870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5052,9 +5052,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5341,10 +5338,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1846"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A645" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A339" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N651" sqref="N651"/>
+      <selection pane="bottomLeft" activeCell="I459" sqref="I459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -18400,8 +18397,8 @@
       <c r="S339" s="7"/>
       <c r="T339" s="7"/>
       <c r="U339" s="7"/>
-      <c r="V339" s="34" t="s">
-        <v>1241</v>
+      <c r="V339" s="35" t="s">
+        <v>1535</v>
       </c>
     </row>
     <row r="340" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18508,7 +18505,7 @@
       <c r="T342" s="7"/>
       <c r="U342" s="7"/>
       <c r="V342" s="34" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="343" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18615,7 +18612,7 @@
       <c r="T345" s="7"/>
       <c r="U345" s="7"/>
       <c r="V345" s="34" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="346" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18722,7 +18719,7 @@
       <c r="T348" s="7"/>
       <c r="U348" s="7"/>
       <c r="V348" s="34" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="349" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18829,7 +18826,7 @@
       <c r="T351" s="7"/>
       <c r="U351" s="7"/>
       <c r="V351" s="34" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="352" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18866,7 +18863,7 @@
       <c r="T352" s="7"/>
       <c r="U352" s="7"/>
       <c r="V352" s="34" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="353" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19206,7 +19203,7 @@
       <c r="T361" s="7"/>
       <c r="U361" s="7"/>
       <c r="V361" s="34" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="362" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19279,8 +19276,8 @@
       <c r="S363" s="7"/>
       <c r="T363" s="7"/>
       <c r="U363" s="7"/>
-      <c r="V363" s="34" t="s">
-        <v>1241</v>
+      <c r="V363" s="35" t="s">
+        <v>1535</v>
       </c>
     </row>
     <row r="364" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19390,7 +19387,7 @@
       <c r="T366" s="7"/>
       <c r="U366" s="7"/>
       <c r="V366" s="34" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="367" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19464,7 +19461,7 @@
       <c r="T368" s="7"/>
       <c r="U368" s="7"/>
       <c r="V368" s="34" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="369" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19502,7 +19499,7 @@
       <c r="T369" s="7"/>
       <c r="U369" s="7"/>
       <c r="V369" s="34" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="370" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19684,7 +19681,7 @@
       <c r="T374" s="7"/>
       <c r="U374" s="7"/>
       <c r="V374" s="34" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="375" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19792,7 +19789,7 @@
       <c r="T377" s="7"/>
       <c r="U377" s="7"/>
       <c r="V377" s="34" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="378" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19938,7 +19935,7 @@
       <c r="T381" s="7"/>
       <c r="U381" s="7"/>
       <c r="V381" s="34" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="382" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19975,7 +19972,7 @@
       <c r="T382" s="7"/>
       <c r="U382" s="7"/>
       <c r="V382" s="34" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="383" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20190,8 +20187,8 @@
       <c r="S388" s="7"/>
       <c r="T388" s="7"/>
       <c r="U388" s="7"/>
-      <c r="V388" s="34" t="s">
-        <v>1241</v>
+      <c r="V388" s="35" t="s">
+        <v>1535</v>
       </c>
     </row>
     <row r="389" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20298,7 +20295,7 @@
       <c r="T391" s="7"/>
       <c r="U391" s="7"/>
       <c r="V391" s="34" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="392" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20440,7 +20437,7 @@
       <c r="T395" s="7"/>
       <c r="U395" s="7"/>
       <c r="V395" s="34" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="396" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20656,7 +20653,7 @@
       <c r="T401" s="7"/>
       <c r="U401" s="7"/>
       <c r="V401" s="34" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="402" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20693,7 +20690,7 @@
       <c r="T402" s="7"/>
       <c r="U402" s="7"/>
       <c r="V402" s="34" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="403" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20730,7 +20727,7 @@
       <c r="T403" s="7"/>
       <c r="U403" s="7"/>
       <c r="V403" s="34" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="404" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20837,7 +20834,7 @@
       <c r="T406" s="7"/>
       <c r="U406" s="7"/>
       <c r="V406" s="34" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="407" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20874,7 +20871,7 @@
       <c r="T407" s="7"/>
       <c r="U407" s="7"/>
       <c r="V407" s="34" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="408" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21052,8 +21049,8 @@
       <c r="S412" s="7"/>
       <c r="T412" s="7"/>
       <c r="U412" s="7"/>
-      <c r="V412" s="34" t="s">
-        <v>1241</v>
+      <c r="V412" s="35" t="s">
+        <v>1535</v>
       </c>
     </row>
     <row r="413" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21160,7 +21157,7 @@
       <c r="T415" s="7"/>
       <c r="U415" s="7"/>
       <c r="V415" s="34" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="416" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21372,7 +21369,7 @@
       <c r="T421" s="7"/>
       <c r="U421" s="7"/>
       <c r="V421" s="34" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="422" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21444,7 +21441,7 @@
       <c r="T423" s="7"/>
       <c r="U423" s="7"/>
       <c r="V423" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="424" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21481,7 +21478,7 @@
       <c r="T424" s="7"/>
       <c r="U424" s="7"/>
       <c r="V424" s="34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="425" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21800,8 +21797,8 @@
       <c r="S433" s="7"/>
       <c r="T433" s="7"/>
       <c r="U433" s="7"/>
-      <c r="V433" s="34" t="s">
-        <v>1241</v>
+      <c r="V433" s="35" t="s">
+        <v>1535</v>
       </c>
     </row>
     <row r="434" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21910,7 +21907,7 @@
       <c r="T436" s="7"/>
       <c r="U436" s="7"/>
       <c r="V436" s="34" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="437" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21947,7 +21944,7 @@
       <c r="T437" s="7"/>
       <c r="U437" s="7"/>
       <c r="V437" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="438" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21984,7 +21981,7 @@
       <c r="T438" s="7"/>
       <c r="U438" s="7"/>
       <c r="V438" s="34" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="439" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22021,7 +22018,7 @@
       <c r="T439" s="7"/>
       <c r="U439" s="7"/>
       <c r="V439" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="440" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22058,7 +22055,7 @@
       <c r="T440" s="7"/>
       <c r="U440" s="7"/>
       <c r="V440" s="34" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="441" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22095,7 +22092,7 @@
       <c r="T441" s="7"/>
       <c r="U441" s="7"/>
       <c r="V441" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="442" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22132,7 +22129,7 @@
       <c r="T442" s="7"/>
       <c r="U442" s="7"/>
       <c r="V442" s="34" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="443" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22169,7 +22166,7 @@
       <c r="T443" s="7"/>
       <c r="U443" s="7"/>
       <c r="V443" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="444" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22241,7 +22238,7 @@
       <c r="T445" s="7"/>
       <c r="U445" s="7"/>
       <c r="V445" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="446" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22313,7 +22310,7 @@
       <c r="T447" s="7"/>
       <c r="U447" s="7"/>
       <c r="V447" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="448" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22420,7 +22417,7 @@
       <c r="T450" s="7"/>
       <c r="U450" s="7"/>
       <c r="V450" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="451" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22492,7 +22489,7 @@
       <c r="T452" s="7"/>
       <c r="U452" s="7"/>
       <c r="V452" s="34" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="453" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22564,7 +22561,7 @@
       <c r="T454" s="7"/>
       <c r="U454" s="7"/>
       <c r="V454" s="34" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="455" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22742,8 +22739,8 @@
       <c r="S459" s="7"/>
       <c r="T459" s="7"/>
       <c r="U459" s="7"/>
-      <c r="V459" s="34" t="s">
-        <v>1241</v>
+      <c r="V459" s="35" t="s">
+        <v>1535</v>
       </c>
     </row>
     <row r="460" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22853,7 +22850,7 @@
       <c r="T462" s="7"/>
       <c r="U462" s="7"/>
       <c r="V462" s="34" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="463" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22999,7 +22996,7 @@
         <v>71</v>
       </c>
       <c r="V466" s="34" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="467" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23109,7 +23106,7 @@
       <c r="T469" s="7"/>
       <c r="U469" s="7"/>
       <c r="V469" s="34" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="470" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23691,7 +23688,7 @@
       <c r="T484" s="7"/>
       <c r="U484" s="7"/>
       <c r="V484" s="34" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="485" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23769,7 +23766,7 @@
       <c r="T486" s="7"/>
       <c r="U486" s="7"/>
       <c r="V486" s="34" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="487" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23965,7 +23962,7 @@
       <c r="T491" s="7"/>
       <c r="U491" s="7"/>
       <c r="V491" s="34" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="492" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24214,7 +24211,7 @@
       <c r="T498" s="7"/>
       <c r="U498" s="7"/>
       <c r="V498" s="34" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="499" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24286,7 +24283,7 @@
       <c r="T500" s="7"/>
       <c r="U500" s="7"/>
       <c r="V500" s="34" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="501" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24926,7 +24923,7 @@
       <c r="T518" s="7"/>
       <c r="U518" s="7"/>
       <c r="V518" s="34" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="519" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25488,7 +25485,7 @@
       <c r="T534" s="7"/>
       <c r="U534" s="7"/>
       <c r="V534" s="34" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="535" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25630,7 +25627,7 @@
       <c r="T538" s="7"/>
       <c r="U538" s="7"/>
       <c r="V538" s="34" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="539" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25912,7 +25909,7 @@
       <c r="T546" s="7"/>
       <c r="U546" s="7"/>
       <c r="V546" s="34" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="547" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26124,7 +26121,7 @@
       <c r="T552" s="7"/>
       <c r="U552" s="7"/>
       <c r="V552" s="34" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="553" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26196,7 +26193,7 @@
       <c r="T554" s="7"/>
       <c r="U554" s="7"/>
       <c r="V554" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="555" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26624,7 +26621,7 @@
       <c r="T566" s="7"/>
       <c r="U566" s="7"/>
       <c r="V566" s="34" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="567" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26698,7 +26695,7 @@
       <c r="T568" s="7"/>
       <c r="U568" s="7"/>
       <c r="V568" s="34" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="569" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26840,7 +26837,7 @@
       <c r="T572" s="7"/>
       <c r="U572" s="7"/>
       <c r="V572" s="34" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="573" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26912,7 +26909,7 @@
       <c r="T574" s="7"/>
       <c r="U574" s="7"/>
       <c r="V574" s="34" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="575" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27056,7 +27053,7 @@
       <c r="T578" s="7"/>
       <c r="U578" s="7"/>
       <c r="V578" s="34" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="579" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27388,7 +27385,7 @@
       <c r="T587" s="7"/>
       <c r="U587" s="7"/>
       <c r="V587" s="34" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="588" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28061,7 +28058,7 @@
       <c r="T605" s="7"/>
       <c r="U605" s="7"/>
       <c r="V605" s="35" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="606" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28098,7 +28095,7 @@
       <c r="T606" s="7"/>
       <c r="U606" s="7"/>
       <c r="V606" s="34" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="607" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28135,7 +28132,7 @@
       <c r="T607" s="7"/>
       <c r="U607" s="7"/>
       <c r="V607" s="35" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="608" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28172,7 +28169,7 @@
       <c r="T608" s="7"/>
       <c r="U608" s="7"/>
       <c r="V608" s="34" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="609" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28209,7 +28206,7 @@
       <c r="T609" s="7"/>
       <c r="U609" s="7"/>
       <c r="V609" s="34" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="610" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28531,7 +28528,7 @@
       <c r="T618" s="7"/>
       <c r="U618" s="7"/>
       <c r="V618" s="34" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="619" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28708,7 +28705,7 @@
       <c r="T623" s="7"/>
       <c r="U623" s="7"/>
       <c r="V623" s="34" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="624" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28885,7 +28882,7 @@
       <c r="T628" s="7"/>
       <c r="U628" s="7"/>
       <c r="V628" s="34" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="629" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29028,7 +29025,7 @@
       <c r="T632" s="13"/>
       <c r="U632" s="13"/>
       <c r="V632" s="34" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="633" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29170,7 +29167,7 @@
       <c r="T636" s="7"/>
       <c r="U636" s="7"/>
       <c r="V636" s="34" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="637" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29312,7 +29309,7 @@
       <c r="T640" s="7"/>
       <c r="U640" s="7"/>
       <c r="V640" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="641" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29683,7 +29680,7 @@
         <v>71</v>
       </c>
       <c r="V650" s="34" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="651" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29797,7 +29794,7 @@
       <c r="T653" s="7"/>
       <c r="U653" s="7"/>
       <c r="V653" s="34" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="654" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -30490,7 +30487,7 @@
       <c r="T673" s="7"/>
       <c r="U673" s="7"/>
       <c r="V673" s="34" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="674" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30589,7 +30586,7 @@
       <c r="T676" s="7"/>
       <c r="U676" s="7"/>
       <c r="V676" s="34" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="677" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30657,7 +30654,7 @@
       <c r="T678" s="7"/>
       <c r="U678" s="7"/>
       <c r="V678" s="34" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="679" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31057,7 +31054,7 @@
       <c r="T690" s="7"/>
       <c r="U690" s="7"/>
       <c r="V690" s="34" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="691" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34033,7 +34030,7 @@
       <c r="T779" s="7"/>
       <c r="U779" s="7"/>
       <c r="V779" s="34" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="780" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34202,7 +34199,7 @@
       <c r="T784" s="7"/>
       <c r="U784" s="7"/>
       <c r="V784" s="34" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="785" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34272,7 +34269,7 @@
       <c r="T786" s="7"/>
       <c r="U786" s="7"/>
       <c r="V786" s="34" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="787" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34307,7 +34304,7 @@
       <c r="T787" s="7"/>
       <c r="U787" s="7"/>
       <c r="V787" s="34" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="788" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34375,7 +34372,7 @@
       <c r="T789" s="7"/>
       <c r="U789" s="7"/>
       <c r="V789" s="34" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="790" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34410,7 +34407,7 @@
       <c r="T790" s="7"/>
       <c r="U790" s="7"/>
       <c r="V790" s="34" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="791" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34445,7 +34442,7 @@
       <c r="S791" s="7"/>
       <c r="T791" s="7"/>
       <c r="V791" s="34" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="792" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34614,7 +34611,7 @@
       <c r="T796" s="7"/>
       <c r="U796" s="7"/>
       <c r="V796" s="34" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="797" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34649,7 +34646,7 @@
       <c r="T797" s="7"/>
       <c r="U797" s="7"/>
       <c r="V797" s="34" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="798" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34717,7 +34714,7 @@
       <c r="T799" s="7"/>
       <c r="U799" s="7"/>
       <c r="V799" s="34" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="800" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34787,7 +34784,7 @@
       <c r="T801" s="7"/>
       <c r="U801" s="7"/>
       <c r="V801" s="34" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="802" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34859,7 +34856,7 @@
       <c r="T803" s="7"/>
       <c r="U803" s="7"/>
       <c r="V803" s="34" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="804" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34927,7 +34924,7 @@
       <c r="T805" s="7"/>
       <c r="U805" s="7"/>
       <c r="V805" s="34" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="806" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34962,7 +34959,7 @@
       <c r="T806" s="7"/>
       <c r="U806" s="7"/>
       <c r="V806" s="34" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="807" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34997,7 +34994,7 @@
       <c r="T807" s="7"/>
       <c r="U807" s="7"/>
       <c r="V807" s="34" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="808" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35098,7 +35095,7 @@
       <c r="T810" s="7"/>
       <c r="U810" s="7"/>
       <c r="V810" s="34" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="811" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35166,7 +35163,7 @@
       <c r="T812" s="7"/>
       <c r="U812" s="7"/>
       <c r="V812" s="34" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="813" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35201,7 +35198,7 @@
       <c r="T813" s="7"/>
       <c r="U813" s="7"/>
       <c r="V813" s="34" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="814" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35236,7 +35233,7 @@
       <c r="T814" s="7"/>
       <c r="U814" s="7"/>
       <c r="V814" s="34" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="815" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35309,7 +35306,7 @@
       <c r="T816" s="7"/>
       <c r="U816" s="7"/>
       <c r="V816" s="34" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="817" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35474,7 +35471,7 @@
       <c r="T821" s="7"/>
       <c r="U821" s="7"/>
       <c r="V821" s="34" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="822" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35775,7 +35772,7 @@
       <c r="T830" s="7"/>
       <c r="U830" s="7"/>
       <c r="V830" s="34" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="831" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35944,7 +35941,7 @@
       <c r="T835" s="7"/>
       <c r="U835" s="7"/>
       <c r="V835" s="34" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="836" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36078,7 +36075,7 @@
       <c r="T839" s="7"/>
       <c r="U839" s="7"/>
       <c r="V839" s="34" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="840" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36383,7 +36380,7 @@
       <c r="T848" s="7"/>
       <c r="U848" s="7"/>
       <c r="V848" s="34" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="849" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36751,7 +36748,7 @@
       <c r="T859" s="7"/>
       <c r="U859" s="7"/>
       <c r="V859" s="34" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="860" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36852,7 +36849,7 @@
       <c r="T862" s="7"/>
       <c r="U862" s="7"/>
       <c r="V862" s="34" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="863" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37051,7 +37048,7 @@
       <c r="T868" s="7"/>
       <c r="U868" s="7"/>
       <c r="V868" s="34" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="869" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37086,7 +37083,7 @@
       <c r="T869" s="7"/>
       <c r="U869" s="7"/>
       <c r="V869" s="34" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="870" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37154,7 +37151,7 @@
       <c r="T871" s="7"/>
       <c r="U871" s="7"/>
       <c r="V871" s="34" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="872" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37355,7 +37352,7 @@
       <c r="T877" s="7"/>
       <c r="U877" s="7"/>
       <c r="V877" s="34" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="878" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37456,7 +37453,7 @@
       <c r="T880" s="7"/>
       <c r="U880" s="7"/>
       <c r="V880" s="34" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="881" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37689,7 +37686,7 @@
       <c r="T887" s="7"/>
       <c r="U887" s="7"/>
       <c r="V887" s="34" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="888" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37823,7 +37820,7 @@
       <c r="T891" s="7"/>
       <c r="U891" s="7"/>
       <c r="V891" s="34" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="892" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38023,7 +38020,7 @@
       <c r="T897" s="7"/>
       <c r="U897" s="7"/>
       <c r="V897" s="34" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="898" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38058,7 +38055,7 @@
       <c r="T898" s="7"/>
       <c r="U898" s="7"/>
       <c r="V898" s="34" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="899" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38126,7 +38123,7 @@
       <c r="T900" s="7"/>
       <c r="U900" s="7"/>
       <c r="V900" s="34" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="901" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38365,7 +38362,7 @@
       <c r="T907" s="7"/>
       <c r="U907" s="7"/>
       <c r="V907" s="34" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="908" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38436,7 +38433,7 @@
       <c r="T909" s="7"/>
       <c r="U909" s="7"/>
       <c r="V909" s="34" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="910" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38507,7 +38504,7 @@
       <c r="T911" s="7"/>
       <c r="U911" s="7"/>
       <c r="V911" s="34" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="912" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38543,7 +38540,7 @@
       <c r="T912" s="7"/>
       <c r="U912" s="7"/>
       <c r="V912" s="34" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="913" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38643,7 +38640,7 @@
       <c r="T915" s="7"/>
       <c r="U915" s="7"/>
       <c r="V915" s="34" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="916" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38711,7 +38708,7 @@
       <c r="T917" s="7"/>
       <c r="U917" s="7"/>
       <c r="V917" s="34" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="918" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38746,7 +38743,7 @@
       <c r="T918" s="7"/>
       <c r="U918" s="7"/>
       <c r="V918" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="919" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38814,7 +38811,7 @@
       <c r="T920" s="7"/>
       <c r="U920" s="7"/>
       <c r="V920" s="34" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="921" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39035,7 +39032,7 @@
       </c>
       <c r="U926" s="7"/>
       <c r="V926" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="927" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39103,7 +39100,7 @@
       <c r="T928" s="7"/>
       <c r="U928" s="7"/>
       <c r="V928" s="34" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="929" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39311,7 +39308,7 @@
       </c>
       <c r="U934" s="7"/>
       <c r="V934" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="935" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39379,7 +39376,7 @@
       <c r="T936" s="7"/>
       <c r="U936" s="7"/>
       <c r="V936" s="34" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="937" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39447,7 +39444,7 @@
       <c r="T938" s="7"/>
       <c r="U938" s="7"/>
       <c r="V938" s="34" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="939" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39548,7 +39545,7 @@
       <c r="T941" s="7"/>
       <c r="U941" s="7"/>
       <c r="V941" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="942" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39616,7 +39613,7 @@
       <c r="T943" s="7"/>
       <c r="U943" s="7"/>
       <c r="V943" s="34" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="944" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39783,7 +39780,7 @@
       <c r="T948" s="7"/>
       <c r="U948" s="7"/>
       <c r="V948" s="34" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="949" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39851,7 +39848,7 @@
       <c r="T950" s="7"/>
       <c r="U950" s="7"/>
       <c r="V950" s="34" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="951" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40018,7 +40015,7 @@
       <c r="T955" s="7"/>
       <c r="U955" s="7"/>
       <c r="V955" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="956" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40086,7 +40083,7 @@
       <c r="T957" s="7"/>
       <c r="U957" s="7"/>
       <c r="V957" s="34" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="958" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40220,7 +40217,7 @@
       <c r="T961" s="7"/>
       <c r="U961" s="7"/>
       <c r="V961" s="34" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="962" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40255,7 +40252,7 @@
       <c r="T962" s="7"/>
       <c r="U962" s="7"/>
       <c r="V962" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="963" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40322,7 +40319,7 @@
       <c r="T964" s="7"/>
       <c r="U964" s="7"/>
       <c r="V964" s="34" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="965" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40489,7 +40486,7 @@
       <c r="T969" s="7"/>
       <c r="U969" s="7"/>
       <c r="V969" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="970" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40557,7 +40554,7 @@
       <c r="T971" s="7"/>
       <c r="U971" s="7"/>
       <c r="V971" s="34" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="972" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40724,7 +40721,7 @@
       <c r="T976" s="7"/>
       <c r="U976" s="7"/>
       <c r="V976" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="977" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40792,7 +40789,7 @@
       <c r="T978" s="7"/>
       <c r="U978" s="7"/>
       <c r="V978" s="34" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="979" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40860,7 +40857,7 @@
       <c r="T980" s="7"/>
       <c r="U980" s="7"/>
       <c r="V980" s="34" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="981" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40928,7 +40925,7 @@
       <c r="T982" s="7"/>
       <c r="U982" s="7"/>
       <c r="V982" s="34" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="983" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40963,7 +40960,7 @@
       <c r="T983" s="7"/>
       <c r="U983" s="7"/>
       <c r="V983" s="34" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="984" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41033,7 +41030,7 @@
       <c r="T985" s="7"/>
       <c r="U985" s="7"/>
       <c r="V985" s="34" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="986" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41103,7 +41100,7 @@
       <c r="T987" s="7"/>
       <c r="U987" s="7"/>
       <c r="V987" s="34" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="988" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41238,7 +41235,7 @@
       <c r="T991" s="7"/>
       <c r="U991" s="7"/>
       <c r="V991" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="992" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41306,7 +41303,7 @@
       <c r="T993" s="7"/>
       <c r="U993" s="7"/>
       <c r="V993" s="34" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="994" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41506,7 +41503,7 @@
       <c r="T999" s="7"/>
       <c r="U999" s="7"/>
       <c r="V999" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="1000" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41574,7 +41571,7 @@
       <c r="T1001" s="7"/>
       <c r="U1001" s="7"/>
       <c r="V1001" s="34" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1002" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41784,7 +41781,7 @@
       <c r="T1007" s="7"/>
       <c r="U1007" s="7"/>
       <c r="V1007" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="1008" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41852,7 +41849,7 @@
       <c r="T1009" s="7"/>
       <c r="U1009" s="7"/>
       <c r="V1009" s="34" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="1010" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41921,7 +41918,7 @@
       <c r="T1011" s="7"/>
       <c r="U1011" s="7"/>
       <c r="V1011" s="34" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="1012" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42267,7 +42264,7 @@
       <c r="T1021" s="7"/>
       <c r="U1021" s="7"/>
       <c r="V1021" s="34" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="1022" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42340,7 +42337,7 @@
       <c r="T1023" s="7"/>
       <c r="U1023" s="7"/>
       <c r="V1023" s="34" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1024" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42512,7 +42509,7 @@
       <c r="T1028" s="7"/>
       <c r="U1028" s="7"/>
       <c r="V1028" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="1029" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42580,7 +42577,7 @@
       <c r="T1030" s="7"/>
       <c r="U1030" s="7"/>
       <c r="V1030" s="34" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="1031" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42648,7 +42645,7 @@
       <c r="T1032" s="7"/>
       <c r="U1032" s="7"/>
       <c r="V1032" s="34" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="1033" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42848,7 +42845,7 @@
       <c r="T1038" s="7"/>
       <c r="U1038" s="7"/>
       <c r="V1038" s="34" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="1039" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42918,7 +42915,7 @@
       <c r="T1040" s="7"/>
       <c r="U1040" s="7"/>
       <c r="V1040" s="34" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="1041" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43054,7 +43051,7 @@
       <c r="T1044" s="7"/>
       <c r="U1044" s="7"/>
       <c r="V1044" s="34" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="1045" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43122,7 +43119,7 @@
       <c r="T1046" s="7"/>
       <c r="U1046" s="7"/>
       <c r="V1046" s="34" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="1047" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43160,7 +43157,7 @@
       <c r="T1047" s="7"/>
       <c r="U1047" s="7"/>
       <c r="V1047" s="34" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="1048" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43373,7 +43370,7 @@
       <c r="T1053" s="7"/>
       <c r="U1053" s="7"/>
       <c r="V1053" s="34" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="1054" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43513,7 +43510,7 @@
       <c r="T1057" s="7"/>
       <c r="U1057" s="7"/>
       <c r="V1057" s="34" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="1058" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43614,7 +43611,7 @@
       <c r="T1060" s="7"/>
       <c r="U1060" s="7"/>
       <c r="V1060" s="34" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="1061" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43781,7 +43778,7 @@
       <c r="T1065" s="7"/>
       <c r="U1065" s="7"/>
       <c r="V1065" s="34" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="1066" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43816,7 +43813,7 @@
       <c r="T1066" s="7"/>
       <c r="U1066" s="7"/>
       <c r="V1066" s="34" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="1067" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43884,7 +43881,7 @@
       <c r="T1068" s="7"/>
       <c r="U1068" s="7"/>
       <c r="V1068" s="34" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="1069" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44022,7 +44019,7 @@
       <c r="T1072" s="7"/>
       <c r="U1072" s="7"/>
       <c r="V1072" s="34" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="1073" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44057,7 +44054,7 @@
       <c r="T1073" s="7"/>
       <c r="U1073" s="7"/>
       <c r="V1073" s="34" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="1074" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44160,7 +44157,7 @@
       <c r="T1076" s="7"/>
       <c r="U1076" s="7"/>
       <c r="V1076" s="34" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="1077" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44228,7 +44225,7 @@
       <c r="T1078" s="7"/>
       <c r="U1078" s="7"/>
       <c r="V1078" s="34" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="1079" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44265,7 +44262,7 @@
         <v>122</v>
       </c>
       <c r="V1079" s="34" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="1080" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44303,7 +44300,7 @@
       <c r="T1080" s="7"/>
       <c r="U1080" s="7"/>
       <c r="V1080" s="34" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="1081" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44377,7 +44374,7 @@
     </row>
     <row r="1083" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1083" s="61" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="H1083" s="43" t="s">
         <v>78</v>
@@ -44737,7 +44734,7 @@
       <c r="T1092" s="7"/>
       <c r="U1092" s="7"/>
       <c r="V1092" s="34" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="1093" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44773,7 +44770,7 @@
       <c r="T1093" s="7"/>
       <c r="U1093" s="7"/>
       <c r="V1093" s="34" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="1094" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45044,7 +45041,7 @@
       <c r="T1101" s="7"/>
       <c r="U1101" s="7"/>
       <c r="V1101" s="34" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="1102" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45080,7 +45077,7 @@
       <c r="T1102" s="7"/>
       <c r="U1102" s="7"/>
       <c r="V1102" s="34" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="1103" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45321,7 +45318,7 @@
       <c r="T1109" s="7"/>
       <c r="U1109" s="7"/>
       <c r="V1109" s="34" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="1110" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45455,7 +45452,7 @@
       <c r="T1113" s="7"/>
       <c r="U1113" s="7"/>
       <c r="V1113" s="34" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="1114" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45694,7 +45691,7 @@
       <c r="T1120" s="7"/>
       <c r="U1120" s="7"/>
       <c r="V1120" s="34" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="1121" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45730,7 +45727,7 @@
       <c r="T1121" s="7"/>
       <c r="U1121" s="7"/>
       <c r="V1121" s="34" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="1122" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46035,7 +46032,7 @@
       <c r="T1130" s="7"/>
       <c r="U1130" s="7"/>
       <c r="V1130" s="34" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="1131" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46186,7 +46183,7 @@
       <c r="T1134" s="7"/>
       <c r="U1134" s="7"/>
       <c r="V1134" s="34" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="1135" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46357,7 +46354,7 @@
       <c r="T1139" s="7"/>
       <c r="U1139" s="7"/>
       <c r="V1139" s="34" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="1140" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46526,7 +46523,7 @@
       <c r="T1144" s="7"/>
       <c r="U1144" s="7"/>
       <c r="V1144" s="34" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="1145" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46629,7 +46626,7 @@
       <c r="T1147" s="7"/>
       <c r="U1147" s="7"/>
       <c r="V1147" s="34" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="1148" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46769,7 +46766,7 @@
       <c r="T1151" s="7"/>
       <c r="U1151" s="7"/>
       <c r="V1151" s="34" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="1152" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46805,7 +46802,7 @@
       <c r="T1152" s="7"/>
       <c r="U1152" s="7"/>
       <c r="V1152" s="34" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="1153" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46913,7 +46910,7 @@
       <c r="T1155" s="7"/>
       <c r="U1155" s="7"/>
       <c r="V1155" s="34" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="1156" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47185,7 +47182,7 @@
       <c r="T1163" s="7"/>
       <c r="U1163" s="7"/>
       <c r="V1163" s="34" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="1164" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47356,7 +47353,7 @@
       <c r="T1168" s="7"/>
       <c r="U1168" s="7"/>
       <c r="V1168" s="34" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="1169" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47461,7 +47458,7 @@
       <c r="T1171" s="7"/>
       <c r="U1171" s="7"/>
       <c r="V1171" s="34" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="1172" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47496,7 +47493,7 @@
       <c r="T1172" s="7"/>
       <c r="U1172" s="7"/>
       <c r="V1172" s="34" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="1173" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47696,7 +47693,7 @@
       <c r="T1178" s="7"/>
       <c r="U1178" s="7"/>
       <c r="V1178" s="34" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="1179" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47999,7 +47996,7 @@
       <c r="T1187" s="7"/>
       <c r="U1187" s="7"/>
       <c r="V1187" s="34" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="1188" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48034,7 +48031,7 @@
       <c r="T1188" s="7"/>
       <c r="U1188" s="7"/>
       <c r="V1188" s="34" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="1189" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48069,7 +48066,7 @@
       <c r="T1189" s="7"/>
       <c r="U1189" s="7"/>
       <c r="V1189" s="34" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="1190" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48306,7 +48303,7 @@
       <c r="T1196" s="7"/>
       <c r="U1196" s="7"/>
       <c r="V1196" s="34" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="1197" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48406,7 +48403,7 @@
       <c r="T1199" s="7"/>
       <c r="U1199" s="7"/>
       <c r="V1199" s="34" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="1200" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48715,7 +48712,7 @@
       <c r="T1208" s="7"/>
       <c r="U1208" s="7"/>
       <c r="V1208" s="34" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="1209" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48816,7 +48813,7 @@
       <c r="T1211" s="7"/>
       <c r="U1211" s="7"/>
       <c r="V1211" s="34" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="1212" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48851,7 +48848,7 @@
       <c r="T1212" s="7"/>
       <c r="U1212" s="7"/>
       <c r="V1212" s="34" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="1213" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48919,7 +48916,7 @@
       <c r="T1214" s="7"/>
       <c r="U1214" s="7"/>
       <c r="V1214" s="34" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="1215" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49020,7 +49017,7 @@
       <c r="T1217" s="7"/>
       <c r="U1217" s="7"/>
       <c r="V1217" s="34" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="1218" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49121,7 +49118,7 @@
       <c r="T1220" s="7"/>
       <c r="U1220" s="7"/>
       <c r="V1220" s="34" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="1221" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49431,7 +49428,7 @@
       <c r="T1229" s="7"/>
       <c r="U1229" s="7"/>
       <c r="V1229" s="34" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="1230" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49501,7 +49498,7 @@
       <c r="T1231" s="7"/>
       <c r="U1231" s="7"/>
       <c r="V1231" s="34" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="1232" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49672,7 +49669,7 @@
       <c r="T1236" s="7"/>
       <c r="U1236" s="7"/>
       <c r="V1236" s="34" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="1237" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49775,7 +49772,7 @@
       <c r="T1239" s="7"/>
       <c r="U1239" s="7"/>
       <c r="V1239" s="34" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="1240" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49876,7 +49873,7 @@
       <c r="T1242" s="7"/>
       <c r="U1242" s="7"/>
       <c r="V1242" s="34" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="1243" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49944,7 +49941,7 @@
       <c r="T1244" s="7"/>
       <c r="U1244" s="7"/>
       <c r="V1244" s="34" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="1245" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50047,7 +50044,7 @@
       <c r="T1247" s="7"/>
       <c r="U1247" s="7"/>
       <c r="V1247" s="34" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="1248" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50180,7 +50177,7 @@
       <c r="T1251" s="7"/>
       <c r="U1251" s="7"/>
       <c r="V1251" s="34" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="1252" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50314,7 +50311,7 @@
       <c r="T1255" s="7"/>
       <c r="U1255" s="7"/>
       <c r="V1255" s="34" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="1256" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50448,7 +50445,7 @@
       <c r="T1259" s="7"/>
       <c r="U1259" s="7"/>
       <c r="V1259" s="34" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="1260" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50650,7 +50647,7 @@
       <c r="T1265" s="7"/>
       <c r="U1265" s="7"/>
       <c r="V1265" s="34" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="1266" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50751,7 +50748,7 @@
       <c r="T1268" s="7"/>
       <c r="U1268" s="7"/>
       <c r="V1268" s="34" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="1269" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50892,7 +50889,7 @@
       <c r="T1272" s="7"/>
       <c r="U1272" s="7"/>
       <c r="V1272" s="34" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="1273" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51059,7 +51056,7 @@
       <c r="T1277" s="7"/>
       <c r="U1277" s="7"/>
       <c r="V1277" s="34" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="1278" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51094,7 +51091,7 @@
       <c r="T1278" s="7"/>
       <c r="U1278" s="7"/>
       <c r="V1278" s="34" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="1279" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51129,7 +51126,7 @@
       <c r="T1279" s="7"/>
       <c r="U1279" s="7"/>
       <c r="V1279" s="34" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="1280" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51310,7 +51307,7 @@
       <c r="T1284" s="7"/>
       <c r="U1284" s="7"/>
       <c r="V1284" s="34" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="1285" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51380,7 +51377,7 @@
       <c r="T1286" s="7"/>
       <c r="U1286" s="7"/>
       <c r="V1286" s="34" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="1287" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51481,7 +51478,7 @@
       <c r="T1289" s="7"/>
       <c r="U1289" s="7"/>
       <c r="V1289" s="34" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="1290" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51703,7 +51700,7 @@
       <c r="T1295" s="7"/>
       <c r="U1295" s="7"/>
       <c r="V1295" s="34" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="1296" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52060,7 +52057,7 @@
       <c r="T1305" s="7"/>
       <c r="U1305" s="7"/>
       <c r="V1305" s="34" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="1306" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52164,7 +52161,7 @@
       <c r="T1308" s="7"/>
       <c r="U1308" s="7"/>
       <c r="V1308" s="34" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="1309" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52461,7 +52458,7 @@
       <c r="T1316" s="7"/>
       <c r="U1316" s="7"/>
       <c r="V1316" s="34" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="1317" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52775,7 +52772,7 @@
       <c r="T1325" s="7"/>
       <c r="U1325" s="7"/>
       <c r="V1325" s="34" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="1326" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52812,7 +52809,7 @@
       <c r="T1326" s="7"/>
       <c r="U1326" s="7"/>
       <c r="V1326" s="34" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="1327" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52849,7 +52846,7 @@
       <c r="T1327" s="7"/>
       <c r="U1327" s="7"/>
       <c r="V1327" s="34" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="1328" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52921,7 +52918,7 @@
       <c r="T1329" s="7"/>
       <c r="U1329" s="7"/>
       <c r="V1329" s="34" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="1330" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53096,7 +53093,7 @@
       <c r="S1334" s="7"/>
       <c r="T1334" s="7"/>
       <c r="V1334" s="34" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="1335" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53133,7 +53130,7 @@
       <c r="S1335" s="7"/>
       <c r="T1335" s="7"/>
       <c r="V1335" s="34" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="1336" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53449,7 +53446,7 @@
       <c r="T1344" s="7"/>
       <c r="U1344" s="7"/>
       <c r="V1344" s="34" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="1345" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53485,7 +53482,7 @@
       <c r="T1345" s="7"/>
       <c r="U1345" s="7"/>
       <c r="V1345" s="34" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="1346" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53627,7 +53624,7 @@
       <c r="T1349" s="7"/>
       <c r="U1349" s="7"/>
       <c r="V1349" s="34" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="1350" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53839,7 +53836,7 @@
       <c r="T1355" s="7"/>
       <c r="U1355" s="7"/>
       <c r="V1355" s="34" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="1356" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53875,7 +53872,7 @@
       <c r="T1356" s="7"/>
       <c r="U1356" s="7"/>
       <c r="V1356" s="34" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="1357" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54289,7 +54286,7 @@
       <c r="T1368" s="7"/>
       <c r="U1368" s="7"/>
       <c r="V1368" s="34" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="1369" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54467,7 +54464,7 @@
       <c r="T1373" s="7"/>
       <c r="U1373" s="7"/>
       <c r="V1373" s="34" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1374" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54538,7 +54535,7 @@
       <c r="T1375" s="7"/>
       <c r="U1375" s="7"/>
       <c r="V1375" s="34" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="1376" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55021,7 +55018,7 @@
       <c r="T1389" s="7"/>
       <c r="U1389" s="7"/>
       <c r="V1389" s="34" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="1390" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55091,7 +55088,7 @@
       <c r="T1391" s="7"/>
       <c r="U1391" s="7"/>
       <c r="V1391" s="34" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="1392" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55299,7 +55296,7 @@
       <c r="T1397" s="7"/>
       <c r="U1397" s="7"/>
       <c r="V1397" s="34" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="1398" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55369,7 +55366,7 @@
       <c r="T1399" s="7"/>
       <c r="U1399" s="7"/>
       <c r="V1399" s="34" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="1400" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55578,7 +55575,7 @@
       <c r="T1405" s="7"/>
       <c r="U1405" s="7"/>
       <c r="V1405" s="34" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="1406" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55789,7 +55786,7 @@
       <c r="T1411" s="7"/>
       <c r="U1411" s="7"/>
       <c r="V1411" s="34" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="1412" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55994,7 +55991,7 @@
       <c r="T1417" s="7"/>
       <c r="U1417" s="7"/>
       <c r="V1417" s="34" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="1418" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56064,7 +56061,7 @@
       <c r="T1419" s="7"/>
       <c r="U1419" s="7"/>
       <c r="V1419" s="34" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="1420" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56134,7 +56131,7 @@
       <c r="T1421" s="7"/>
       <c r="U1421" s="7"/>
       <c r="V1421" s="34" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1422" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56646,7 +56643,7 @@
       <c r="T1436" s="7"/>
       <c r="U1436" s="7"/>
       <c r="V1436" s="34" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="1437" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56716,7 +56713,7 @@
       <c r="T1438" s="7"/>
       <c r="U1438" s="7"/>
       <c r="V1438" s="34" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="1439" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56786,7 +56783,7 @@
       <c r="T1440" s="7"/>
       <c r="U1440" s="7"/>
       <c r="V1440" s="34" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="1441" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56924,7 +56921,7 @@
       <c r="T1444" s="7"/>
       <c r="U1444" s="7"/>
       <c r="V1444" s="34" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="1445" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57290,7 +57287,7 @@
       <c r="T1454" s="7"/>
       <c r="U1454" s="7"/>
       <c r="V1454" s="34" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="1455" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57328,7 +57325,7 @@
       <c r="T1455" s="7"/>
       <c r="U1455" s="7"/>
       <c r="V1455" s="34" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="1456" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57404,7 +57401,7 @@
       <c r="T1457" s="7"/>
       <c r="U1457" s="7"/>
       <c r="V1457" s="34" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="1458" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57557,7 +57554,7 @@
       <c r="T1461" s="10"/>
       <c r="U1461" s="7"/>
       <c r="V1461" s="34" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="1462" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57708,7 +57705,7 @@
       <c r="T1465" s="7"/>
       <c r="U1465" s="7"/>
       <c r="V1465" s="34" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="1466" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57862,7 +57859,7 @@
       <c r="T1469" s="7"/>
       <c r="U1469" s="7"/>
       <c r="V1469" s="34" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="1470" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58010,7 +58007,7 @@
       <c r="T1473" s="7"/>
       <c r="U1473" s="7"/>
       <c r="V1473" s="34" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="1474" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58048,7 +58045,7 @@
       <c r="T1474" s="7"/>
       <c r="U1474" s="7"/>
       <c r="V1474" s="35" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="1475" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58198,7 +58195,7 @@
       <c r="T1478" s="7"/>
       <c r="U1478" s="7"/>
       <c r="V1478" s="34" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="1479" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58637,7 +58634,7 @@
       <c r="T1490" s="7"/>
       <c r="U1490" s="7"/>
       <c r="V1490" s="34" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="1491" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58814,7 +58811,7 @@
         <f t="shared" si="71"/>
         <v>46</v>
       </c>
-      <c r="N1495" s="62" t="s">
+      <c r="N1495" s="34" t="s">
         <v>875</v>
       </c>
       <c r="O1495" s="6"/>
@@ -58853,7 +58850,7 @@
         <f t="shared" si="71"/>
         <v>47</v>
       </c>
-      <c r="N1496" s="62" t="s">
+      <c r="N1496" s="34" t="s">
         <v>876</v>
       </c>
       <c r="O1496" s="6"/>
@@ -58981,7 +58978,7 @@
       <c r="T1499" s="7"/>
       <c r="U1499" s="7"/>
       <c r="V1499" s="34" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="1500" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59350,7 +59347,7 @@
         <v>113</v>
       </c>
       <c r="V1509" s="34" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="1510" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59381,7 +59378,7 @@
         <f t="shared" si="71"/>
         <v>61</v>
       </c>
-      <c r="N1510" s="63" t="s">
+      <c r="N1510" s="62" t="s">
         <v>270</v>
       </c>
       <c r="O1510" s="6"/>
@@ -59427,7 +59424,7 @@
         <f t="shared" si="71"/>
         <v>62</v>
       </c>
-      <c r="N1511" s="63" t="s">
+      <c r="N1511" s="62" t="s">
         <v>885</v>
       </c>
       <c r="O1511" s="6"/>
@@ -59518,7 +59515,7 @@
       <c r="T1513" s="7"/>
       <c r="U1513" s="7"/>
       <c r="V1513" s="34" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="1514" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59562,7 +59559,7 @@
         <v>113</v>
       </c>
       <c r="V1514" s="34" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="1515" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59679,7 +59676,7 @@
       <c r="T1517" s="7"/>
       <c r="U1517" s="7"/>
       <c r="V1517" s="34" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="1518" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59717,7 +59714,7 @@
       <c r="T1518" s="7"/>
       <c r="U1518" s="7"/>
       <c r="V1518" s="34" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="1519" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59793,7 +59790,7 @@
       <c r="T1520" s="7"/>
       <c r="U1520" s="7"/>
       <c r="V1520" s="34" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="1521" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59903,12 +59900,12 @@
       <c r="T1523" s="7"/>
       <c r="U1523" s="7"/>
       <c r="V1523" s="34" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="1524" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1524" s="61" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="C1524" s="7" t="s">
         <v>87</v>
@@ -59986,7 +59983,7 @@
       <c r="T1525" s="7"/>
       <c r="U1525" s="7"/>
       <c r="V1525" s="34" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="1526" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60105,7 +60102,7 @@
       <c r="T1528" s="7"/>
       <c r="U1528" s="7"/>
       <c r="V1528" s="34" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="1529" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60325,7 +60322,7 @@
       <c r="T1534" s="7"/>
       <c r="U1534" s="7"/>
       <c r="V1534" s="34" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="1535" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60435,7 +60432,7 @@
       <c r="T1537" s="7"/>
       <c r="U1537" s="7"/>
       <c r="V1537" s="34" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="1538" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60545,7 +60542,7 @@
       <c r="T1540" s="7"/>
       <c r="U1540" s="7"/>
       <c r="V1540" s="34" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="1541" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60583,7 +60580,7 @@
       <c r="T1541" s="7"/>
       <c r="U1541" s="7"/>
       <c r="V1541" s="34" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="1542" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60765,7 +60762,7 @@
       <c r="T1546" s="7"/>
       <c r="U1546" s="7"/>
       <c r="V1546" s="34" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="1547" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60914,7 +60911,7 @@
       <c r="T1550" s="7"/>
       <c r="U1550" s="7"/>
       <c r="V1550" s="34" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="1551" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60988,7 +60985,7 @@
       <c r="T1552" s="7"/>
       <c r="U1552" s="7"/>
       <c r="V1552" s="34" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="1553" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61062,7 +61059,7 @@
       <c r="T1554" s="7"/>
       <c r="U1554" s="7"/>
       <c r="V1554" s="34" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1555" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61446,7 +61443,7 @@
       <c r="T1564" s="7"/>
       <c r="U1564" s="7"/>
       <c r="V1564" s="34" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="1565" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61558,7 +61555,7 @@
       <c r="T1567" s="7"/>
       <c r="U1567" s="7"/>
       <c r="V1567" s="34" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="1568" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61669,7 +61666,7 @@
       <c r="T1570" s="7"/>
       <c r="U1570" s="7"/>
       <c r="V1570" s="34" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="1571" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61745,7 +61742,7 @@
       <c r="T1572" s="7"/>
       <c r="U1572" s="7"/>
       <c r="V1572" s="34" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="1573" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61859,7 +61856,7 @@
       </c>
       <c r="U1575" s="7"/>
       <c r="V1575" s="34" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="1576" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62007,7 +62004,7 @@
       <c r="T1579" s="7"/>
       <c r="U1579" s="7"/>
       <c r="V1579" s="34" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="1580" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62104,7 +62101,7 @@
         <v>19</v>
       </c>
       <c r="V1582" s="34" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="1583" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62136,7 +62133,7 @@
         <v>0</v>
       </c>
       <c r="V1583" s="34" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="1584" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62284,7 +62281,7 @@
         <v>19</v>
       </c>
       <c r="V1588" s="34" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="1589" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62386,7 +62383,7 @@
         <v>19</v>
       </c>
       <c r="V1591" s="34" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="1592" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62534,7 +62531,7 @@
         <v>0</v>
       </c>
       <c r="V1596" s="34" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="1597" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62652,7 +62649,7 @@
         <v>19</v>
       </c>
       <c r="V1600" s="34" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="1601" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62931,7 +62928,7 @@
         <v>19</v>
       </c>
       <c r="V1609" s="34" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="1610" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62963,7 +62960,7 @@
         <v>0</v>
       </c>
       <c r="V1610" s="34" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="1611" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63024,7 +63021,7 @@
         <v>0</v>
       </c>
       <c r="V1612" s="34" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="1613" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63056,7 +63053,7 @@
         <v>0</v>
       </c>
       <c r="V1613" s="34" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="1614" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63088,7 +63085,7 @@
         <v>0</v>
       </c>
       <c r="V1614" s="34" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="1615" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63120,7 +63117,7 @@
         <v>19</v>
       </c>
       <c r="V1615" s="34" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="1616" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63341,7 +63338,7 @@
         <v>0</v>
       </c>
       <c r="V1622" s="34" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="1623" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63402,7 +63399,7 @@
         <v>19</v>
       </c>
       <c r="V1624" s="34" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="1625" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63538,7 +63535,7 @@
     </row>
     <row r="1629" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1629" s="61" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="C1629" s="7" t="s">
         <v>87</v>
@@ -63659,7 +63656,7 @@
         <v>0</v>
       </c>
       <c r="V1631" s="34" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="1632" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63726,7 +63723,7 @@
         <v>19</v>
       </c>
       <c r="V1633" s="34" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="1634" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64000,7 +63997,7 @@
       </c>
       <c r="U1642" s="7"/>
       <c r="V1642" s="34" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="1643" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64380,7 +64377,7 @@
         <v>19</v>
       </c>
       <c r="V1654" s="34" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="1655" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64737,7 +64734,7 @@
         <v>113</v>
       </c>
       <c r="V1666" s="34" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="1667" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64917,7 +64914,7 @@
         <v>19</v>
       </c>
       <c r="V1672" s="34" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="1673" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64981,7 +64978,7 @@
         <v>19</v>
       </c>
       <c r="V1674" s="34" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="1675" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65013,7 +65010,7 @@
         <v>0</v>
       </c>
       <c r="V1675" s="34" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="1676" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65048,7 +65045,7 @@
         <v>113</v>
       </c>
       <c r="V1676" s="34" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="1677" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65080,7 +65077,7 @@
         <v>0</v>
       </c>
       <c r="V1677" s="34" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="1678" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65115,7 +65112,7 @@
         <v>19</v>
       </c>
       <c r="V1678" s="34" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1679" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65147,7 +65144,7 @@
         <v>0</v>
       </c>
       <c r="V1679" s="34" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="1680" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65237,7 +65234,7 @@
         <v>19</v>
       </c>
       <c r="V1682" s="34" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="1683" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65269,7 +65266,7 @@
         <v>0</v>
       </c>
       <c r="V1683" s="34" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="1684" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65452,7 +65449,7 @@
         <v>19</v>
       </c>
       <c r="V1689" s="34" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="1690" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65484,7 +65481,7 @@
         <v>0</v>
       </c>
       <c r="V1690" s="34" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="1691" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65548,7 +65545,7 @@
         <v>122</v>
       </c>
       <c r="V1692" s="34" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="1693" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65667,7 +65664,7 @@
         <v>0</v>
       </c>
       <c r="V1696" s="34" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="1697" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65728,7 +65725,7 @@
         <v>19</v>
       </c>
       <c r="V1698" s="34" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="1699" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65760,7 +65757,7 @@
         <v>0</v>
       </c>
       <c r="V1699" s="34" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="1700" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65791,7 +65788,7 @@
         <v>19</v>
       </c>
       <c r="V1700" s="34" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="1701" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66044,7 +66041,7 @@
         <v>0</v>
       </c>
       <c r="V1708" s="34" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="1709" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66076,7 +66073,7 @@
         <v>19</v>
       </c>
       <c r="V1709" s="34" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="1710" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66224,7 +66221,7 @@
         <v>0</v>
       </c>
       <c r="V1714" s="34" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="1715" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66285,7 +66282,7 @@
         <v>19</v>
       </c>
       <c r="V1716" s="34" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="1717" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66439,7 +66436,7 @@
         <v>0</v>
       </c>
       <c r="V1721" s="34" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="1722" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66567,7 +66564,7 @@
         <v>19</v>
       </c>
       <c r="V1725" s="34" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="1726" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66721,7 +66718,7 @@
         <v>19</v>
       </c>
       <c r="V1730" s="34" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="1731" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66753,7 +66750,7 @@
         <v>18</v>
       </c>
       <c r="V1731" s="34" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="1732" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66818,7 +66815,7 @@
       </c>
       <c r="U1733" s="7"/>
       <c r="V1733" s="34" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="1734" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66949,7 +66946,7 @@
         <v>0</v>
       </c>
       <c r="V1737" s="34" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="1738" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66981,7 +66978,7 @@
         <v>19</v>
       </c>
       <c r="V1738" s="34" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="1739" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67147,7 +67144,7 @@
         <v>19</v>
       </c>
       <c r="V1743" s="34" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="1744" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67327,7 +67324,7 @@
         <v>19</v>
       </c>
       <c r="V1749" s="34" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="1750" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67463,7 +67460,7 @@
         <v>19</v>
       </c>
       <c r="V1753" s="34" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="1754" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67643,7 +67640,7 @@
         <v>0</v>
       </c>
       <c r="V1759" s="34" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="1760" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67733,7 +67730,7 @@
         <v>19</v>
       </c>
       <c r="V1762" s="34" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="1763" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67794,7 +67791,7 @@
         <v>0</v>
       </c>
       <c r="V1764" s="34" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="1765" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67971,7 +67968,7 @@
         <v>0</v>
       </c>
       <c r="V1770" s="34" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="1771" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68006,7 +68003,7 @@
         <v>19</v>
       </c>
       <c r="V1771" s="34" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="1772" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68363,7 +68360,7 @@
         <v>19</v>
       </c>
       <c r="V1783" s="34" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="1784" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68482,7 +68479,7 @@
         <v>0</v>
       </c>
       <c r="V1787" s="34" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="1788" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68543,7 +68540,7 @@
         <v>0</v>
       </c>
       <c r="V1789" s="34" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="1790" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68604,7 +68601,7 @@
         <v>19</v>
       </c>
       <c r="V1791" s="34" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="1792" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68636,7 +68633,7 @@
         <v>0</v>
       </c>
       <c r="V1792" s="34" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="1793" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68899,7 +68896,7 @@
         <v>19</v>
       </c>
       <c r="V1801" s="34" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="1802" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69177,7 +69174,7 @@
       <c r="T1810" s="7"/>
       <c r="U1810" s="7"/>
       <c r="V1810" s="34" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="1811" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69214,7 +69211,7 @@
         <v>94</v>
       </c>
       <c r="V1811" s="34" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="1812" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69246,7 +69243,7 @@
         <v>0</v>
       </c>
       <c r="V1812" s="34" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="1813" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69278,7 +69275,7 @@
         <v>0</v>
       </c>
       <c r="V1813" s="34" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="1814" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69368,7 +69365,7 @@
         <v>19</v>
       </c>
       <c r="V1816" s="34" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="1817" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69400,7 +69397,7 @@
         <v>0</v>
       </c>
       <c r="V1817" s="34" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="1818" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69435,7 +69432,7 @@
         <v>19</v>
       </c>
       <c r="V1818" s="34" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="1819" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69644,7 +69641,7 @@
         <v>19</v>
       </c>
       <c r="V1825" s="34" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="1826" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69734,7 +69731,7 @@
         <v>19</v>
       </c>
       <c r="V1828" s="34" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="1829" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69766,7 +69763,7 @@
         <v>17</v>
       </c>
       <c r="V1829" s="34" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="1830" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70121,7 +70118,7 @@
         <v>0</v>
       </c>
       <c r="V1840" s="34" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="1841" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70211,7 +70208,7 @@
         <v>0</v>
       </c>
       <c r="V1843" s="34" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="1844" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70272,7 +70269,7 @@
         <v>19</v>
       </c>
       <c r="V1845" s="34" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="1846" spans="3:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 04 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3941EC2D-6D85-4461-8428-3E7B2DB3FBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC0AFE4-A83C-4E7B-BA64-A966D2DC12AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6824" uniqueCount="1536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6822" uniqueCount="1536">
   <si>
     <t>PS</t>
   </si>
@@ -5342,9 +5342,9 @@
   <dimension ref="A1:V1846"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1209" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U1090" sqref="U1090"/>
+      <selection pane="bottomLeft" activeCell="U1226" sqref="U1226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -48614,9 +48614,7 @@
       <c r="R1205" s="7"/>
       <c r="S1205" s="7"/>
       <c r="T1205" s="7"/>
-      <c r="U1205" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="U1205" s="7"/>
       <c r="V1205" s="34" t="s">
         <v>1176</v>
       </c>
@@ -49329,9 +49327,7 @@
       <c r="R1226" s="7"/>
       <c r="S1226" s="7"/>
       <c r="T1226" s="7"/>
-      <c r="U1226" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="U1226" s="7"/>
       <c r="V1226" s="34" t="s">
         <v>1176</v>
       </c>

</xml_diff>

<commit_message>
nmv 30 03 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF6AE65-E845-4A32-A8CE-7F7E6A8291C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF4F19B-8EF7-4457-8AC8-3D52626D2949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6819" uniqueCount="1537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6822" uniqueCount="1537">
   <si>
     <t>PS</t>
   </si>
@@ -4272,9 +4272,6 @@
     <t>vaqyaqskRuditi# vayaH - kRut</t>
   </si>
   <si>
-    <t>viShpa#rdhAq itiq viH - spaqrddhAqH</t>
-  </si>
-  <si>
     <t>dUqroqhaqNamiti# duH - roqhaqNam</t>
   </si>
   <si>
@@ -4299,9 +4296,6 @@
     <t>svaqnIqketi# su - aqnIqkaq</t>
   </si>
   <si>
-    <t>saqndRugeti# saM - dRuk</t>
-  </si>
-  <si>
     <t>cAruqritiq cAru#H</t>
   </si>
   <si>
@@ -4639,6 +4633,12 @@
   </si>
   <si>
     <t>svaqnIqkaq</t>
+  </si>
+  <si>
+    <t>viShpa#rdhAq itiq vi - spaqrddhAqH</t>
+  </si>
+  <si>
+    <t>saqndRugiti# saM - dRuk</t>
   </si>
 </sst>
 </file>
@@ -5347,10 +5347,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1846"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1468" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1459" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1473" sqref="N1473"/>
+      <selection pane="bottomLeft" activeCell="V1474" sqref="V1474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -17897,7 +17897,7 @@
         <v>1</v>
       </c>
       <c r="N325" s="35" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
       <c r="O325" s="7" t="s">
         <v>0</v>
@@ -17909,7 +17909,7 @@
       <c r="T325" s="7"/>
       <c r="U325" s="7"/>
       <c r="V325" s="35" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="326" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18407,7 +18407,7 @@
       <c r="T339" s="7"/>
       <c r="U339" s="7"/>
       <c r="V339" s="35" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="340" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19286,7 +19286,7 @@
       <c r="T363" s="7"/>
       <c r="U363" s="7"/>
       <c r="V363" s="35" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="364" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20197,7 +20197,7 @@
       <c r="T388" s="7"/>
       <c r="U388" s="7"/>
       <c r="V388" s="35" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="389" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20831,7 +20831,7 @@
         <v>82</v>
       </c>
       <c r="N406" s="35" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="O406" s="7" t="s">
         <v>0</v>
@@ -21059,7 +21059,7 @@
       <c r="T412" s="7"/>
       <c r="U412" s="7"/>
       <c r="V412" s="35" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="413" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21807,7 +21807,7 @@
       <c r="T433" s="7"/>
       <c r="U433" s="7"/>
       <c r="V433" s="35" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="434" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22749,7 +22749,7 @@
       <c r="T459" s="7"/>
       <c r="U459" s="7"/>
       <c r="V459" s="35" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="460" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23975,7 +23975,7 @@
       <c r="T491" s="7"/>
       <c r="U491" s="7"/>
       <c r="V491" s="35" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="492" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -42590,7 +42590,7 @@
       <c r="T1030" s="7"/>
       <c r="U1030" s="7"/>
       <c r="V1030" s="35" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="1031" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43826,7 +43826,7 @@
       <c r="T1066" s="7"/>
       <c r="U1066" s="7"/>
       <c r="V1066" s="35" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="1067" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44387,7 +44387,7 @@
     </row>
     <row r="1083" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1083" s="61" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="H1083" s="43" t="s">
         <v>78</v>
@@ -46033,7 +46033,7 @@
         <v>83</v>
       </c>
       <c r="N1130" s="35" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="O1130" s="7" t="s">
         <v>0</v>
@@ -56791,8 +56791,8 @@
       <c r="S1440" s="7"/>
       <c r="T1440" s="7"/>
       <c r="U1440" s="7"/>
-      <c r="V1440" s="34" t="s">
-        <v>1414</v>
+      <c r="V1440" s="35" t="s">
+        <v>1535</v>
       </c>
     </row>
     <row r="1441" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56930,7 +56930,7 @@
       <c r="T1444" s="7"/>
       <c r="U1444" s="7"/>
       <c r="V1444" s="34" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="1445" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57296,7 +57296,7 @@
       <c r="T1454" s="7"/>
       <c r="U1454" s="7"/>
       <c r="V1454" s="34" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1455" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57334,7 +57334,7 @@
       <c r="T1455" s="7"/>
       <c r="U1455" s="7"/>
       <c r="V1455" s="34" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="1456" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57410,7 +57410,7 @@
       <c r="T1457" s="7"/>
       <c r="U1457" s="7"/>
       <c r="V1457" s="34" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="1458" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57563,7 +57563,7 @@
       <c r="T1461" s="10"/>
       <c r="U1461" s="7"/>
       <c r="V1461" s="34" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="1462" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57714,7 +57714,7 @@
       <c r="T1465" s="7"/>
       <c r="U1465" s="7"/>
       <c r="V1465" s="34" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="1466" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57868,7 +57868,7 @@
       <c r="T1469" s="7"/>
       <c r="U1469" s="7"/>
       <c r="V1469" s="34" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="1470" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58004,7 +58004,7 @@
         <v>24</v>
       </c>
       <c r="N1473" s="35" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="O1473" s="7" t="s">
         <v>0</v>
@@ -58016,7 +58016,7 @@
       <c r="T1473" s="7"/>
       <c r="U1473" s="7"/>
       <c r="V1473" s="34" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="1474" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58054,7 +58054,7 @@
       <c r="T1474" s="7"/>
       <c r="U1474" s="7"/>
       <c r="V1474" s="35" t="s">
-        <v>1423</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="1475" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58204,7 +58204,7 @@
       <c r="T1478" s="7"/>
       <c r="U1478" s="7"/>
       <c r="V1478" s="34" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="1479" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58643,7 +58643,7 @@
       <c r="T1490" s="7"/>
       <c r="U1490" s="7"/>
       <c r="V1490" s="34" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="1491" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58987,7 +58987,7 @@
       <c r="T1499" s="7"/>
       <c r="U1499" s="7"/>
       <c r="V1499" s="34" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="1500" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59356,7 +59356,7 @@
         <v>113</v>
       </c>
       <c r="V1509" s="34" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1510" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59524,7 +59524,7 @@
       <c r="T1513" s="7"/>
       <c r="U1513" s="7"/>
       <c r="V1513" s="34" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="1514" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59685,7 +59685,7 @@
       <c r="T1517" s="7"/>
       <c r="U1517" s="7"/>
       <c r="V1517" s="34" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="1518" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59723,7 +59723,7 @@
       <c r="T1518" s="7"/>
       <c r="U1518" s="7"/>
       <c r="V1518" s="34" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="1519" spans="2:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59799,7 +59799,7 @@
       <c r="T1520" s="7"/>
       <c r="U1520" s="7"/>
       <c r="V1520" s="34" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="1521" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59909,12 +59909,12 @@
       <c r="T1523" s="7"/>
       <c r="U1523" s="7"/>
       <c r="V1523" s="34" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="1524" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1524" s="61" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="C1524" s="7" t="s">
         <v>87</v>
@@ -59992,7 +59992,7 @@
       <c r="T1525" s="7"/>
       <c r="U1525" s="7"/>
       <c r="V1525" s="34" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="1526" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60111,7 +60111,7 @@
       <c r="T1528" s="7"/>
       <c r="U1528" s="7"/>
       <c r="V1528" s="34" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="1529" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60331,7 +60331,7 @@
       <c r="T1534" s="7"/>
       <c r="U1534" s="7"/>
       <c r="V1534" s="34" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="1535" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60441,7 +60441,7 @@
       <c r="T1537" s="7"/>
       <c r="U1537" s="7"/>
       <c r="V1537" s="34" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="1538" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60551,7 +60551,7 @@
       <c r="T1540" s="7"/>
       <c r="U1540" s="7"/>
       <c r="V1540" s="34" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="1541" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60589,7 +60589,7 @@
       <c r="T1541" s="7"/>
       <c r="U1541" s="7"/>
       <c r="V1541" s="34" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="1542" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60771,7 +60771,7 @@
       <c r="T1546" s="7"/>
       <c r="U1546" s="7"/>
       <c r="V1546" s="34" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="1547" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60920,7 +60920,7 @@
       <c r="T1550" s="7"/>
       <c r="U1550" s="7"/>
       <c r="V1550" s="34" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="1551" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60994,7 +60994,7 @@
       <c r="T1552" s="7"/>
       <c r="U1552" s="7"/>
       <c r="V1552" s="34" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="1553" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61068,7 +61068,7 @@
       <c r="T1554" s="7"/>
       <c r="U1554" s="7"/>
       <c r="V1554" s="34" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="1555" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61452,7 +61452,7 @@
       <c r="T1564" s="7"/>
       <c r="U1564" s="7"/>
       <c r="V1564" s="34" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="1565" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61564,7 +61564,7 @@
       <c r="T1567" s="7"/>
       <c r="U1567" s="7"/>
       <c r="V1567" s="34" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="1568" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61675,7 +61675,7 @@
       <c r="T1570" s="7"/>
       <c r="U1570" s="7"/>
       <c r="V1570" s="34" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="1571" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61751,7 +61751,7 @@
       <c r="T1572" s="7"/>
       <c r="U1572" s="7"/>
       <c r="V1572" s="34" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="1573" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61865,7 +61865,7 @@
       </c>
       <c r="U1575" s="7"/>
       <c r="V1575" s="34" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="1576" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62013,7 +62013,7 @@
       <c r="T1579" s="7"/>
       <c r="U1579" s="7"/>
       <c r="V1579" s="34" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="1580" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62110,7 +62110,7 @@
         <v>19</v>
       </c>
       <c r="V1582" s="34" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="1583" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62142,7 +62142,7 @@
         <v>0</v>
       </c>
       <c r="V1583" s="34" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="1584" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62290,7 +62290,7 @@
         <v>19</v>
       </c>
       <c r="V1588" s="34" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="1589" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62392,7 +62392,7 @@
         <v>19</v>
       </c>
       <c r="V1591" s="34" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="1592" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62540,7 +62540,7 @@
         <v>0</v>
       </c>
       <c r="V1596" s="34" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="1597" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62658,7 +62658,7 @@
         <v>19</v>
       </c>
       <c r="V1600" s="34" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="1601" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62937,7 +62937,7 @@
         <v>19</v>
       </c>
       <c r="V1609" s="34" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="1610" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62969,7 +62969,7 @@
         <v>0</v>
       </c>
       <c r="V1610" s="34" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="1611" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63030,7 +63030,7 @@
         <v>0</v>
       </c>
       <c r="V1612" s="34" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1613" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63062,7 +63062,7 @@
         <v>0</v>
       </c>
       <c r="V1613" s="34" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="1614" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63094,7 +63094,7 @@
         <v>0</v>
       </c>
       <c r="V1614" s="34" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="1615" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63126,7 +63126,7 @@
         <v>19</v>
       </c>
       <c r="V1615" s="34" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="1616" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63347,7 +63347,7 @@
         <v>0</v>
       </c>
       <c r="V1622" s="34" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="1623" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63408,7 +63408,7 @@
         <v>19</v>
       </c>
       <c r="V1624" s="34" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="1625" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63544,7 +63544,7 @@
     </row>
     <row r="1629" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1629" s="61" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="C1629" s="7" t="s">
         <v>87</v>
@@ -63665,7 +63665,7 @@
         <v>0</v>
       </c>
       <c r="V1631" s="34" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="1632" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63732,7 +63732,7 @@
         <v>19</v>
       </c>
       <c r="V1633" s="34" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="1634" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64006,7 +64006,7 @@
       </c>
       <c r="U1642" s="7"/>
       <c r="V1642" s="34" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="1643" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64290,7 +64290,7 @@
         <v>68</v>
       </c>
       <c r="T1651" s="1" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="V1651" s="34" t="s">
         <v>1169</v>
@@ -64392,7 +64392,7 @@
         <v>19</v>
       </c>
       <c r="V1654" s="34" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="1655" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64749,7 +64749,7 @@
         <v>113</v>
       </c>
       <c r="V1666" s="34" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="1667" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64833,7 +64833,7 @@
         <v>220</v>
       </c>
       <c r="N1669" s="35" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="V1669" s="34" t="s">
         <v>1169</v>
@@ -64929,7 +64929,7 @@
         <v>19</v>
       </c>
       <c r="V1672" s="34" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="1673" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64993,7 +64993,7 @@
         <v>19</v>
       </c>
       <c r="V1674" s="34" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="1675" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65025,7 +65025,7 @@
         <v>0</v>
       </c>
       <c r="V1675" s="34" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="1676" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65060,7 +65060,7 @@
         <v>113</v>
       </c>
       <c r="V1676" s="34" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="1677" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65092,7 +65092,7 @@
         <v>0</v>
       </c>
       <c r="V1677" s="34" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="1678" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65127,7 +65127,7 @@
         <v>19</v>
       </c>
       <c r="V1678" s="34" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="1679" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65159,7 +65159,7 @@
         <v>0</v>
       </c>
       <c r="V1679" s="34" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="1680" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65249,7 +65249,7 @@
         <v>19</v>
       </c>
       <c r="V1682" s="34" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="1683" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65281,7 +65281,7 @@
         <v>0</v>
       </c>
       <c r="V1683" s="34" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="1684" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65464,7 +65464,7 @@
         <v>19</v>
       </c>
       <c r="V1689" s="34" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="1690" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65496,7 +65496,7 @@
         <v>0</v>
       </c>
       <c r="V1690" s="34" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="1691" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65560,7 +65560,7 @@
         <v>121</v>
       </c>
       <c r="V1692" s="34" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="1693" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65679,7 +65679,7 @@
         <v>0</v>
       </c>
       <c r="V1696" s="34" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="1697" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65740,7 +65740,7 @@
         <v>19</v>
       </c>
       <c r="V1698" s="34" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="1699" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65772,7 +65772,7 @@
         <v>0</v>
       </c>
       <c r="V1699" s="34" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="1700" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65803,7 +65803,7 @@
         <v>19</v>
       </c>
       <c r="V1700" s="34" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="1701" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66056,7 +66056,7 @@
         <v>0</v>
       </c>
       <c r="V1708" s="34" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="1709" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66088,7 +66088,7 @@
         <v>19</v>
       </c>
       <c r="V1709" s="34" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="1710" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66236,7 +66236,7 @@
         <v>0</v>
       </c>
       <c r="V1714" s="34" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="1715" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66297,7 +66297,7 @@
         <v>19</v>
       </c>
       <c r="V1716" s="34" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="1717" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66384,7 +66384,7 @@
         <v>270</v>
       </c>
       <c r="N1719" s="56" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="O1719" s="54"/>
       <c r="P1719" s="64"/>
@@ -66452,7 +66452,7 @@
         <v>0</v>
       </c>
       <c r="V1721" s="34" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1722" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66580,7 +66580,7 @@
         <v>19</v>
       </c>
       <c r="V1725" s="34" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="1726" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66725,7 +66725,7 @@
         <v>281</v>
       </c>
       <c r="N1730" s="35" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="O1730" s="7" t="s">
         <v>0</v>
@@ -66734,7 +66734,7 @@
         <v>19</v>
       </c>
       <c r="V1730" s="34" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="1731" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66766,7 +66766,7 @@
         <v>18</v>
       </c>
       <c r="V1731" s="35" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="1732" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66831,7 +66831,7 @@
       </c>
       <c r="U1733" s="7"/>
       <c r="V1733" s="34" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="1734" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66962,7 +66962,7 @@
         <v>0</v>
       </c>
       <c r="V1737" s="34" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="1738" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66994,7 +66994,7 @@
         <v>19</v>
       </c>
       <c r="V1738" s="34" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="1739" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67160,7 +67160,7 @@
         <v>19</v>
       </c>
       <c r="V1743" s="34" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="1744" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67340,7 +67340,7 @@
         <v>19</v>
       </c>
       <c r="V1749" s="34" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="1750" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67476,7 +67476,7 @@
         <v>19</v>
       </c>
       <c r="V1753" s="34" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="1754" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67656,7 +67656,7 @@
         <v>0</v>
       </c>
       <c r="V1759" s="34" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="1760" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67746,7 +67746,7 @@
         <v>19</v>
       </c>
       <c r="V1762" s="34" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="1763" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67807,7 +67807,7 @@
         <v>0</v>
       </c>
       <c r="V1764" s="34" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="1765" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67984,7 +67984,7 @@
         <v>0</v>
       </c>
       <c r="V1770" s="34" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="1771" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68019,7 +68019,7 @@
         <v>19</v>
       </c>
       <c r="V1771" s="34" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="1772" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68374,7 +68374,7 @@
         <v>19</v>
       </c>
       <c r="V1783" s="34" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="1784" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68493,7 +68493,7 @@
         <v>0</v>
       </c>
       <c r="V1787" s="34" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="1788" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68554,7 +68554,7 @@
         <v>0</v>
       </c>
       <c r="V1789" s="34" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="1790" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68615,7 +68615,7 @@
         <v>19</v>
       </c>
       <c r="V1791" s="34" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="1792" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68647,7 +68647,7 @@
         <v>0</v>
       </c>
       <c r="V1792" s="34" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="1793" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68910,7 +68910,7 @@
         <v>19</v>
       </c>
       <c r="V1801" s="34" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="1802" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69188,7 +69188,7 @@
       <c r="T1810" s="7"/>
       <c r="U1810" s="7"/>
       <c r="V1810" s="34" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="1811" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69225,7 +69225,7 @@
         <v>94</v>
       </c>
       <c r="V1811" s="34" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="1812" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69257,7 +69257,7 @@
         <v>0</v>
       </c>
       <c r="V1812" s="34" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="1813" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69289,7 +69289,7 @@
         <v>0</v>
       </c>
       <c r="V1813" s="34" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="1814" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69379,7 +69379,7 @@
         <v>19</v>
       </c>
       <c r="V1816" s="34" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="1817" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69411,7 +69411,7 @@
         <v>0</v>
       </c>
       <c r="V1817" s="34" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="1818" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69446,7 +69446,7 @@
         <v>19</v>
       </c>
       <c r="V1818" s="34" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="1819" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69655,7 +69655,7 @@
         <v>19</v>
       </c>
       <c r="V1825" s="34" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="1826" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69745,7 +69745,7 @@
         <v>19</v>
       </c>
       <c r="V1828" s="34" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="1829" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69873,7 +69873,7 @@
         <v>383</v>
       </c>
       <c r="N1832" s="35" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="V1832" s="34" t="s">
         <v>1169</v>
@@ -70126,13 +70126,13 @@
         <v>391</v>
       </c>
       <c r="N1840" s="35" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="O1840" s="7" t="s">
         <v>0</v>
       </c>
       <c r="V1840" s="34" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="1841" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70222,7 +70222,7 @@
         <v>0</v>
       </c>
       <c r="V1843" s="34" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="1844" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70283,7 +70283,7 @@
         <v>19</v>
       </c>
       <c r="V1845" s="34" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="1846" spans="3:22" x14ac:dyDescent="0.25">

</xml_diff>